<commit_message>
Resumen Plan Proyecto Issues Leiva
planificación parte Leiva
</commit_message>
<xml_diff>
--- a/Entregables/05 Plantillas/Resumen Plan Proyecto.xlsx
+++ b/Entregables/05 Plantillas/Resumen Plan Proyecto.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juans\Downloads\Inventario-AP-master\Entregables\05 Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7536" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Importantes" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Plan Cuichan" sheetId="5" r:id="rId4"/>
     <sheet name="Plan Leiva" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
@@ -173,7 +173,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
@@ -437,6 +437,9 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -444,9 +447,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -778,37 +778,37 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="23" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="23" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="31"/>
       <c r="B1" s="31"/>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45" t="s">
+      <c r="E1" s="46"/>
+      <c r="F1" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="46"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G1" s="47"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
-      <c r="C2" s="47"/>
+      <c r="C2" s="48"/>
       <c r="D2" s="30" t="s">
         <v>42</v>
       </c>
@@ -822,8 +822,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="45" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="32" t="s">
@@ -845,8 +845,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="48"/>
+    <row r="4" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="45"/>
       <c r="B4" s="34" t="s">
         <v>11</v>
       </c>
@@ -867,8 +867,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="48" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="45" t="s">
         <v>39</v>
       </c>
       <c r="B5" s="32" t="s">
@@ -880,8 +880,8 @@
       <c r="F5" s="44"/>
       <c r="G5" s="44"/>
     </row>
-    <row r="6" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="48"/>
+    <row r="6" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="45"/>
       <c r="B6" s="34" t="s">
         <v>11</v>
       </c>
@@ -895,49 +895,69 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="48" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="45" t="s">
         <v>40</v>
       </c>
       <c r="B7" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="48"/>
+      <c r="C7" s="33">
+        <v>1200</v>
+      </c>
+      <c r="D7" s="33">
+        <v>1100</v>
+      </c>
+      <c r="E7" s="33">
+        <v>20</v>
+      </c>
+      <c r="F7" s="44">
+        <v>3</v>
+      </c>
+      <c r="G7" s="44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="45"/>
       <c r="B8" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C8" s="35">
+        <v>1000</v>
+      </c>
+      <c r="D8" s="35">
+        <v>750</v>
+      </c>
+      <c r="E8" s="35">
+        <v>18</v>
+      </c>
+      <c r="F8" s="39">
+        <v>2</v>
+      </c>
+      <c r="G8" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="31"/>
       <c r="B12" s="31"/>
       <c r="C12" s="36"/>
       <c r="D12" s="36"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="37"/>
       <c r="B13" s="36"/>
       <c r="C13" s="31"/>
       <c r="D13" s="31"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="37"/>
       <c r="B14" s="36"/>
       <c r="C14" s="31"/>
       <c r="D14" s="31"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="31"/>
       <c r="B15" s="31"/>
       <c r="C15" s="31"/>
@@ -964,12 +984,12 @@
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="14.42578125" style="23"/>
+    <col min="1" max="16384" width="14.44140625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -987,7 +1007,7 @@
         <v>43057</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>2</v>
       </c>
@@ -1005,7 +1025,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>5</v>
       </c>
@@ -1023,7 +1043,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
@@ -1043,22 +1063,22 @@
         <v>1965</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="22"/>
       <c r="C6" s="11">
         <f>('Datos Importantes'!D3+'Datos Importantes'!D5+'Datos Importantes'!D7)/('Datos Importantes'!C3+'Datos Importantes'!C5+'Datos Importantes'!C7)</f>
-        <v>0.9</v>
+        <v>0.90740740740740744</v>
       </c>
       <c r="D6" s="40">
         <f>('Datos Importantes'!D4+'Datos Importantes'!D6+'Datos Importantes'!D8)/('Datos Importantes'!C4+'Datos Importantes'!C6+'Datos Importantes'!C8)</f>
-        <v>0.97297297297297303</v>
+        <v>0.86729857819905209</v>
       </c>
       <c r="E6" s="40">
         <f>('Datos Importantes'!D4+'Datos Importantes'!D6+'Datos Importantes'!D8)/('Datos Importantes'!C4+'Datos Importantes'!C6+'Datos Importantes'!C8)</f>
-        <v>0.97297297297297303</v>
+        <v>0.86729857819905209</v>
       </c>
       <c r="F6" s="51"/>
       <c r="G6" s="51"/>
@@ -1066,22 +1086,22 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="22"/>
       <c r="C7" s="11">
         <f>('Datos Importantes'!C3+'Datos Importantes'!C5+'Datos Importantes'!C7)/('Datos Importantes'!E3+'Datos Importantes'!E5+'Datos Importantes'!E7)</f>
-        <v>62.5</v>
+        <v>61.363636363636367</v>
       </c>
       <c r="D7" s="41">
         <f>('Datos Importantes'!C4+'Datos Importantes'!C6+'Datos Importantes'!C8)/('Datos Importantes'!E4+'Datos Importantes'!E6+'Datos Importantes'!E8)</f>
-        <v>61.666666666666664</v>
+        <v>58.611111111111114</v>
       </c>
       <c r="E7" s="41">
         <f>('Datos Importantes'!C4+'Datos Importantes'!C6+'Datos Importantes'!C8)/('Datos Importantes'!E4+'Datos Importantes'!E6+'Datos Importantes'!E8)</f>
-        <v>61.666666666666664</v>
+        <v>58.611111111111114</v>
       </c>
       <c r="F7" s="51"/>
       <c r="G7" s="51"/>
@@ -1090,27 +1110,27 @@
         <v>0.43666666666666665</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="22"/>
       <c r="C8" s="40">
         <f>('Datos Importantes'!F3+'Datos Importantes'!F5+'Datos Importantes'!F7)/(('Datos Importantes'!C3+'Datos Importantes'!C5+'Datos Importantes'!C7)/1000)</f>
-        <v>1.3333333333333333</v>
+        <v>1.8518518518518516</v>
       </c>
       <c r="D8" s="41">
         <f>('Datos Importantes'!F4+'Datos Importantes'!F6+'Datos Importantes'!F8)/(('Datos Importantes'!C4+'Datos Importantes'!C6+'Datos Importantes'!C8)/1000)</f>
-        <v>7.2072072072072064</v>
+        <v>4.7393364928909953</v>
       </c>
       <c r="E8" s="41">
         <f>('Datos Importantes'!F4+'Datos Importantes'!F6+'Datos Importantes'!F8)/(('Datos Importantes'!C4+'Datos Importantes'!C6+'Datos Importantes'!C8)/1000)</f>
-        <v>7.2072072072072064</v>
+        <v>4.7393364928909953</v>
       </c>
       <c r="F8" s="51"/>
       <c r="G8" s="51"/>
     </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
         <v>16</v>
       </c>
@@ -1121,7 +1141,7 @@
       <c r="F9" s="51"/>
       <c r="G9" s="51"/>
     </row>
-    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
         <v>17</v>
       </c>
@@ -1136,22 +1156,22 @@
         <v>32.75</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8">
         <f>'Datos Importantes'!C3+'Datos Importantes'!C5+'Datos Importantes'!C7</f>
-        <v>1500</v>
+        <v>2700</v>
       </c>
       <c r="D11" s="8">
         <f>'Datos Importantes'!C4+'Datos Importantes'!C6+'Datos Importantes'!C8</f>
-        <v>1110</v>
+        <v>2110</v>
       </c>
       <c r="E11" s="8">
         <f>'Datos Importantes'!C4+'Datos Importantes'!C6+'Datos Importantes'!C8</f>
-        <v>1110</v>
+        <v>2110</v>
       </c>
       <c r="F11" s="51"/>
       <c r="G11" s="51"/>
@@ -1160,67 +1180,67 @@
         <v>137.40458015267177</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="49" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="50"/>
       <c r="C12" s="22">
         <f>'Datos Importantes'!C3+'Datos Importantes'!C5+'Datos Importantes'!C7</f>
-        <v>1500</v>
+        <v>2700</v>
       </c>
       <c r="D12" s="22">
         <f>'Datos Importantes'!C4+'Datos Importantes'!C6+'Datos Importantes'!C8</f>
-        <v>1110</v>
+        <v>2110</v>
       </c>
       <c r="E12" s="22">
         <f>'Datos Importantes'!C4+'Datos Importantes'!C6+'Datos Importantes'!C8</f>
-        <v>1110</v>
+        <v>2110</v>
       </c>
       <c r="F12" s="51"/>
       <c r="G12" s="51"/>
     </row>
-    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="22"/>
       <c r="C13" s="42">
         <f>MAX(C11:C12)</f>
-        <v>1500</v>
+        <v>2700</v>
       </c>
       <c r="D13" s="42">
         <f t="shared" ref="D13:E13" si="0">MAX(D11:D12)</f>
-        <v>1110</v>
+        <v>2110</v>
       </c>
       <c r="E13" s="42">
         <f t="shared" si="0"/>
-        <v>1110</v>
+        <v>2110</v>
       </c>
       <c r="F13" s="51"/>
       <c r="G13" s="51"/>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
         <v>21</v>
       </c>
       <c r="B14" s="22"/>
       <c r="C14" s="22">
         <f>MIN(C11:C12)</f>
-        <v>1500</v>
+        <v>2700</v>
       </c>
       <c r="D14" s="22">
         <f t="shared" ref="D14:E14" si="1">MIN(D11:D12)</f>
-        <v>1110</v>
+        <v>2110</v>
       </c>
       <c r="E14" s="22">
         <f t="shared" si="1"/>
-        <v>1110</v>
+        <v>2110</v>
       </c>
       <c r="F14" s="51"/>
       <c r="G14" s="51"/>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>22</v>
       </c>
@@ -1239,7 +1259,7 @@
       </c>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
         <v>24</v>
       </c>
@@ -1262,7 +1282,7 @@
       </c>
       <c r="G16" s="52"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
         <v>25</v>
       </c>
@@ -1285,30 +1305,30 @@
       </c>
       <c r="G17" s="53"/>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>26</v>
       </c>
       <c r="B18" s="22"/>
       <c r="C18" s="22">
         <f>'Plan Andrade'!C18+'Plan Cuichan'!C18+'Plan Leiva'!C18</f>
-        <v>1350</v>
+        <v>2450</v>
       </c>
       <c r="D18" s="22">
         <f>'Plan Andrade'!D18+'Plan Cuichan'!D18+'Plan Leiva'!D18</f>
-        <v>1080</v>
+        <v>1830</v>
       </c>
       <c r="E18" s="22">
         <f>'Plan Andrade'!E18+'Plan Cuichan'!E18+'Plan Leiva'!E18</f>
-        <v>1080</v>
+        <v>1830</v>
       </c>
       <c r="F18" s="29">
         <f>E18/C18</f>
-        <v>0.8</v>
+        <v>0.74693877551020404</v>
       </c>
       <c r="G18" s="53"/>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
         <v>27</v>
       </c>
@@ -1331,7 +1351,7 @@
       </c>
       <c r="G19" s="53"/>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>28</v>
       </c>
@@ -1354,7 +1374,7 @@
       </c>
       <c r="G20" s="53"/>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>29</v>
       </c>
@@ -1377,7 +1397,7 @@
       </c>
       <c r="G21" s="53"/>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
         <v>30</v>
       </c>
@@ -1388,45 +1408,45 @@
       <c r="F22" s="28"/>
       <c r="G22" s="53"/>
     </row>
-    <row r="23" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
         <v>31</v>
       </c>
       <c r="B23" s="22"/>
       <c r="C23" s="22">
         <f>SUM(C16:C22)</f>
-        <v>3150</v>
+        <v>4250</v>
       </c>
       <c r="D23" s="22">
         <f t="shared" ref="D23:E23" si="4">SUM(D16:D22)</f>
-        <v>2730</v>
+        <v>3480</v>
       </c>
       <c r="E23" s="22">
         <f t="shared" si="4"/>
-        <v>2730</v>
+        <v>3480</v>
       </c>
       <c r="F23" s="22"/>
       <c r="G23" s="53"/>
     </row>
-    <row r="24" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
         <v>32</v>
       </c>
       <c r="B24" s="22"/>
       <c r="C24" s="22">
         <f>MAX(C16:C21)</f>
-        <v>1350</v>
+        <v>2450</v>
       </c>
       <c r="D24" s="22">
         <f t="shared" ref="D24:E24" si="5">MAX(D16:D21)</f>
-        <v>1080</v>
+        <v>1830</v>
       </c>
       <c r="E24" s="22">
         <f t="shared" si="5"/>
-        <v>1080</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
         <v>33</v>
       </c>
@@ -1444,7 +1464,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>34</v>
       </c>
@@ -1465,7 +1485,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
         <v>24</v>
       </c>
@@ -1491,7 +1511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="25" t="s">
         <v>25</v>
       </c>
@@ -1517,7 +1537,7 @@
         <v>0.22222222222222221</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="25" t="s">
         <v>26</v>
       </c>
@@ -1540,10 +1560,10 @@
       </c>
       <c r="G29" s="43">
         <f t="shared" si="8"/>
-        <v>0.55555555555555558</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>0.32786885245901637</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
         <v>27</v>
       </c>
@@ -1569,7 +1589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="25" t="s">
         <v>28</v>
       </c>
@@ -1595,7 +1615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
         <v>29</v>
       </c>
@@ -1621,7 +1641,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="25" t="s">
         <v>31</v>
       </c>
@@ -1641,7 +1661,7 @@
       <c r="F33" s="22"/>
       <c r="G33" s="26"/>
     </row>
-    <row r="34" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>36</v>
       </c>
@@ -1662,7 +1682,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
         <v>24</v>
       </c>
@@ -1688,7 +1708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
         <v>25</v>
       </c>
@@ -1714,7 +1734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
         <v>26</v>
       </c>
@@ -1737,10 +1757,10 @@
       </c>
       <c r="G37" s="43">
         <f t="shared" si="11"/>
-        <v>0.27777777777777779</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>0.16393442622950818</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="25" t="s">
         <v>27</v>
       </c>
@@ -1766,7 +1786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="25" t="s">
         <v>28</v>
       </c>
@@ -1792,7 +1812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
         <v>29</v>
       </c>
@@ -1818,7 +1838,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
         <v>31</v>
       </c>
@@ -1858,13 +1878,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
       <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1882,7 +1902,7 @@
         <v>43057</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1900,7 +1920,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1918,7 +1938,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
@@ -1938,7 +1958,7 @@
         <v>1965</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>13</v>
       </c>
@@ -1961,7 +1981,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>14</v>
       </c>
@@ -1985,7 +2005,7 @@
         <v>0.43666666666666665</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>15</v>
       </c>
@@ -2005,7 +2025,7 @@
       <c r="F8" s="51"/>
       <c r="G8" s="51"/>
     </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>16</v>
       </c>
@@ -2016,7 +2036,7 @@
       <c r="F9" s="51"/>
       <c r="G9" s="51"/>
     </row>
-    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>17</v>
       </c>
@@ -2031,7 +2051,7 @@
         <v>32.75</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
@@ -2055,7 +2075,7 @@
         <v>137.40458015267177</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="49" t="s">
         <v>19</v>
       </c>
@@ -2075,7 +2095,7 @@
       <c r="F12" s="51"/>
       <c r="G12" s="51"/>
     </row>
-    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>20</v>
       </c>
@@ -2095,7 +2115,7 @@
       <c r="F13" s="51"/>
       <c r="G13" s="51"/>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>21</v>
       </c>
@@ -2115,7 +2135,7 @@
       <c r="F14" s="51"/>
       <c r="G14" s="51"/>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>22</v>
       </c>
@@ -2134,7 +2154,7 @@
       </c>
       <c r="G15" s="16"/>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>24</v>
       </c>
@@ -2154,7 +2174,7 @@
       </c>
       <c r="G16" s="52"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>25</v>
       </c>
@@ -2174,7 +2194,7 @@
       </c>
       <c r="G17" s="53"/>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>26</v>
       </c>
@@ -2197,7 +2217,7 @@
       </c>
       <c r="G18" s="53"/>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>27</v>
       </c>
@@ -2217,7 +2237,7 @@
       </c>
       <c r="G19" s="53"/>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>28</v>
       </c>
@@ -2237,7 +2257,7 @@
       </c>
       <c r="G20" s="53"/>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>29</v>
       </c>
@@ -2257,7 +2277,7 @@
       </c>
       <c r="G21" s="53"/>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>30</v>
       </c>
@@ -2268,7 +2288,7 @@
       <c r="F22" s="28"/>
       <c r="G22" s="53"/>
     </row>
-    <row r="23" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>31</v>
       </c>
@@ -2288,7 +2308,7 @@
       <c r="F23" s="10"/>
       <c r="G23" s="53"/>
     </row>
-    <row r="24" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>32</v>
       </c>
@@ -2308,7 +2328,7 @@
       <c r="F24" s="23"/>
       <c r="G24" s="23"/>
     </row>
-    <row r="25" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>33</v>
       </c>
@@ -2328,7 +2348,7 @@
       <c r="F25" s="23"/>
       <c r="G25" s="23"/>
     </row>
-    <row r="26" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>34</v>
       </c>
@@ -2349,7 +2369,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>24</v>
       </c>
@@ -2372,7 +2392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>25</v>
       </c>
@@ -2395,7 +2415,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>26</v>
       </c>
@@ -2418,7 +2438,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>27</v>
       </c>
@@ -2441,7 +2461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>28</v>
       </c>
@@ -2464,7 +2484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>29</v>
       </c>
@@ -2487,7 +2507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>31</v>
       </c>
@@ -2507,7 +2527,7 @@
       <c r="F33" s="10"/>
       <c r="G33" s="3"/>
     </row>
-    <row r="34" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>36</v>
       </c>
@@ -2528,7 +2548,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>24</v>
       </c>
@@ -2551,7 +2571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>25</v>
       </c>
@@ -2574,7 +2594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>26</v>
       </c>
@@ -2597,7 +2617,7 @@
         <v>5.5555555555555552E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>27</v>
       </c>
@@ -2620,7 +2640,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>28</v>
       </c>
@@ -2643,7 +2663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>29</v>
       </c>
@@ -2666,7 +2686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
         <v>31</v>
       </c>
@@ -2710,12 +2730,12 @@
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="14.42578125" style="23"/>
+    <col min="1" max="16384" width="14.44140625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -2733,7 +2753,7 @@
         <v>43057</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>2</v>
       </c>
@@ -2751,7 +2771,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>5</v>
       </c>
@@ -2769,7 +2789,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
@@ -2789,7 +2809,7 @@
         <v>1965</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>13</v>
       </c>
@@ -2812,7 +2832,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>14</v>
       </c>
@@ -2836,7 +2856,7 @@
         <v>0.43666666666666665</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
         <v>15</v>
       </c>
@@ -2856,7 +2876,7 @@
       <c r="F8" s="51"/>
       <c r="G8" s="51"/>
     </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
         <v>16</v>
       </c>
@@ -2867,7 +2887,7 @@
       <c r="F9" s="51"/>
       <c r="G9" s="51"/>
     </row>
-    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
         <v>17</v>
       </c>
@@ -2882,7 +2902,7 @@
         <v>32.75</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
@@ -2906,7 +2926,7 @@
         <v>137.40458015267177</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="49" t="s">
         <v>19</v>
       </c>
@@ -2926,7 +2946,7 @@
       <c r="F12" s="51"/>
       <c r="G12" s="51"/>
     </row>
-    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
         <v>20</v>
       </c>
@@ -2946,7 +2966,7 @@
       <c r="F13" s="51"/>
       <c r="G13" s="51"/>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
         <v>21</v>
       </c>
@@ -2966,7 +2986,7 @@
       <c r="F14" s="51"/>
       <c r="G14" s="51"/>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>22</v>
       </c>
@@ -2985,7 +3005,7 @@
       </c>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
         <v>24</v>
       </c>
@@ -3005,7 +3025,7 @@
       </c>
       <c r="G16" s="52"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
         <v>25</v>
       </c>
@@ -3025,7 +3045,7 @@
       </c>
       <c r="G17" s="53"/>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>26</v>
       </c>
@@ -3048,7 +3068,7 @@
       </c>
       <c r="G18" s="53"/>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
         <v>27</v>
       </c>
@@ -3068,7 +3088,7 @@
       </c>
       <c r="G19" s="53"/>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>28</v>
       </c>
@@ -3088,7 +3108,7 @@
       </c>
       <c r="G20" s="53"/>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>29</v>
       </c>
@@ -3108,7 +3128,7 @@
       </c>
       <c r="G21" s="53"/>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
         <v>30</v>
       </c>
@@ -3119,7 +3139,7 @@
       <c r="F22" s="28"/>
       <c r="G22" s="53"/>
     </row>
-    <row r="23" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
         <v>31</v>
       </c>
@@ -3139,7 +3159,7 @@
       <c r="F23" s="22"/>
       <c r="G23" s="53"/>
     </row>
-    <row r="24" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
         <v>32</v>
       </c>
@@ -3157,7 +3177,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
         <v>33</v>
       </c>
@@ -3175,7 +3195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>34</v>
       </c>
@@ -3196,7 +3216,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
         <v>24</v>
       </c>
@@ -3219,7 +3239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="25" t="s">
         <v>25</v>
       </c>
@@ -3242,7 +3262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="25" t="s">
         <v>26</v>
       </c>
@@ -3265,7 +3285,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
         <v>27</v>
       </c>
@@ -3288,7 +3308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="25" t="s">
         <v>28</v>
       </c>
@@ -3311,7 +3331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
         <v>29</v>
       </c>
@@ -3334,7 +3354,7 @@
         <v>1.875</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="25" t="s">
         <v>31</v>
       </c>
@@ -3354,7 +3374,7 @@
       <c r="F33" s="22"/>
       <c r="G33" s="26"/>
     </row>
-    <row r="34" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>36</v>
       </c>
@@ -3375,7 +3395,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
         <v>24</v>
       </c>
@@ -3398,7 +3418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
         <v>25</v>
       </c>
@@ -3421,7 +3441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
         <v>26</v>
       </c>
@@ -3444,7 +3464,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="25" t="s">
         <v>27</v>
       </c>
@@ -3467,7 +3487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="25" t="s">
         <v>28</v>
       </c>
@@ -3490,7 +3510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
         <v>29</v>
       </c>
@@ -3513,7 +3533,7 @@
         <v>1.875</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
         <v>31</v>
       </c>
@@ -3557,12 +3577,12 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="14.42578125" style="23"/>
+    <col min="1" max="16384" width="14.44140625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -3580,7 +3600,7 @@
         <v>43057</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>2</v>
       </c>
@@ -3598,7 +3618,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>5</v>
       </c>
@@ -3616,7 +3636,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
@@ -3636,22 +3656,22 @@
         <v>1965</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="22"/>
-      <c r="C6" s="11" t="e">
+      <c r="C6" s="11">
         <f>'Datos Importantes'!D7/'Datos Importantes'!C7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D6" s="40" t="e">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D6" s="40">
         <f>'Datos Importantes'!D8/'Datos Importantes'!C8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E6" s="40" t="e">
+        <v>0.75</v>
+      </c>
+      <c r="E6" s="40">
         <f>'Datos Importantes'!D8/'Datos Importantes'!C8</f>
-        <v>#DIV/0!</v>
+        <v>0.75</v>
       </c>
       <c r="F6" s="51"/>
       <c r="G6" s="51"/>
@@ -3659,22 +3679,22 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="22"/>
-      <c r="C7" s="11" t="e">
+      <c r="C7" s="11">
         <f>'Datos Importantes'!C7/'Datos Importantes'!E7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D7" s="41" t="e">
+        <v>60</v>
+      </c>
+      <c r="D7" s="41">
         <f>'Datos Importantes'!C8/'Datos Importantes'!E8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E7" s="41" t="e">
+        <v>55.555555555555557</v>
+      </c>
+      <c r="E7" s="41">
         <f>'Datos Importantes'!C8/'Datos Importantes'!E8</f>
-        <v>#DIV/0!</v>
+        <v>55.555555555555557</v>
       </c>
       <c r="F7" s="51"/>
       <c r="G7" s="51"/>
@@ -3683,27 +3703,27 @@
         <v>0.43666666666666665</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="22"/>
-      <c r="C8" s="40" t="e">
+      <c r="C8" s="40">
         <f>'Datos Importantes'!F7/('Datos Importantes'!C7/1000)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D8" s="41" t="e">
+        <v>2.5</v>
+      </c>
+      <c r="D8" s="41">
         <f>'Datos Importantes'!F8/('Datos Importantes'!C8/1000)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E8" s="41" t="e">
+        <v>2</v>
+      </c>
+      <c r="E8" s="41">
         <f>'Datos Importantes'!F8/('Datos Importantes'!C8/1000)</f>
-        <v>#DIV/0!</v>
+        <v>2</v>
       </c>
       <c r="F8" s="51"/>
       <c r="G8" s="51"/>
     </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
         <v>16</v>
       </c>
@@ -3714,7 +3734,7 @@
       <c r="F9" s="51"/>
       <c r="G9" s="51"/>
     </row>
-    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
         <v>17</v>
       </c>
@@ -3729,22 +3749,22 @@
         <v>32.75</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8">
         <f>'Datos Importantes'!C7</f>
-        <v>0</v>
+        <v>1200</v>
       </c>
       <c r="D11" s="8">
         <f>'Datos Importantes'!C8</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="E11" s="8">
         <f>'Datos Importantes'!C8</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="F11" s="51"/>
       <c r="G11" s="51"/>
@@ -3753,67 +3773,67 @@
         <v>137.40458015267177</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="49" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="50"/>
       <c r="C12" s="22">
         <f>'Datos Importantes'!C7</f>
-        <v>0</v>
+        <v>1200</v>
       </c>
       <c r="D12" s="22">
         <f>'Datos Importantes'!C8</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="E12" s="22">
         <f>'Datos Importantes'!C8</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="F12" s="51"/>
       <c r="G12" s="51"/>
     </row>
-    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="22"/>
       <c r="C13" s="42">
         <f>MAX(C11:C12)</f>
-        <v>0</v>
+        <v>1200</v>
       </c>
       <c r="D13" s="42">
         <f t="shared" ref="D13:E13" si="0">MAX(D11:D12)</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="E13" s="42">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="F13" s="51"/>
       <c r="G13" s="51"/>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
         <v>21</v>
       </c>
       <c r="B14" s="22"/>
       <c r="C14" s="22">
         <f>MIN(C11:C12)</f>
-        <v>0</v>
+        <v>1200</v>
       </c>
       <c r="D14" s="22">
         <f t="shared" ref="D14:E14" si="1">MIN(D11:D12)</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="E14" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="F14" s="51"/>
       <c r="G14" s="51"/>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>22</v>
       </c>
@@ -3832,7 +3852,7 @@
       </c>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
         <v>24</v>
       </c>
@@ -3852,7 +3872,7 @@
       </c>
       <c r="G16" s="52"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
         <v>25</v>
       </c>
@@ -3872,30 +3892,30 @@
       </c>
       <c r="G17" s="53"/>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>26</v>
       </c>
       <c r="B18" s="22"/>
       <c r="C18" s="22">
         <f>'Datos Importantes'!D7</f>
-        <v>0</v>
+        <v>1100</v>
       </c>
       <c r="D18" s="22">
         <f>'Datos Importantes'!D8</f>
-        <v>0</v>
+        <v>750</v>
       </c>
       <c r="E18" s="22">
         <f>'Datos Importantes'!D8</f>
-        <v>0</v>
-      </c>
-      <c r="F18" s="29" t="e">
+        <v>750</v>
+      </c>
+      <c r="F18" s="29">
         <f>E18/C18</f>
-        <v>#DIV/0!</v>
+        <v>0.68181818181818177</v>
       </c>
       <c r="G18" s="53"/>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
         <v>27</v>
       </c>
@@ -3915,7 +3935,7 @@
       </c>
       <c r="G19" s="53"/>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>28</v>
       </c>
@@ -3935,7 +3955,7 @@
       </c>
       <c r="G20" s="53"/>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>29</v>
       </c>
@@ -3955,7 +3975,7 @@
       </c>
       <c r="G21" s="53"/>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
         <v>30</v>
       </c>
@@ -3966,63 +3986,63 @@
       <c r="F22" s="28"/>
       <c r="G22" s="53"/>
     </row>
-    <row r="23" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
         <v>31</v>
       </c>
       <c r="B23" s="22"/>
       <c r="C23" s="22">
         <f>SUM(C16:C22)</f>
-        <v>600</v>
+        <v>1700</v>
       </c>
       <c r="D23" s="22">
         <f t="shared" ref="D23:E23" si="4">SUM(D16:D22)</f>
-        <v>550</v>
+        <v>1300</v>
       </c>
       <c r="E23" s="22">
         <f t="shared" si="4"/>
-        <v>550</v>
+        <v>1300</v>
       </c>
       <c r="F23" s="22"/>
       <c r="G23" s="53"/>
     </row>
-    <row r="24" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
         <v>32</v>
       </c>
       <c r="B24" s="22"/>
       <c r="C24" s="22">
         <f>MAX(C16:C21)</f>
-        <v>150</v>
+        <v>1100</v>
       </c>
       <c r="D24" s="22">
         <f t="shared" ref="D24:E24" si="5">MAX(D16:D21)</f>
-        <v>160</v>
+        <v>750</v>
       </c>
       <c r="E24" s="22">
         <f t="shared" si="5"/>
-        <v>160</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
         <v>33</v>
       </c>
       <c r="B25" s="22"/>
       <c r="C25" s="22">
         <f>MIN(C16:C21)</f>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="D25" s="22">
         <f t="shared" ref="D25:E25" si="6">MIN(D16:D21)</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="E25" s="22">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>34</v>
       </c>
@@ -4043,7 +4063,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
         <v>24</v>
       </c>
@@ -4066,7 +4086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="25" t="s">
         <v>25</v>
       </c>
@@ -4089,7 +4109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="25" t="s">
         <v>26</v>
       </c>
@@ -4107,12 +4127,12 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="G29" s="43" t="e">
+      <c r="G29" s="43">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
         <v>27</v>
       </c>
@@ -4135,7 +4155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="25" t="s">
         <v>28</v>
       </c>
@@ -4158,7 +4178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
         <v>29</v>
       </c>
@@ -4181,7 +4201,7 @@
         <v>1.875</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="25" t="s">
         <v>31</v>
       </c>
@@ -4201,7 +4221,7 @@
       <c r="F33" s="22"/>
       <c r="G33" s="26"/>
     </row>
-    <row r="34" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>36</v>
       </c>
@@ -4222,7 +4242,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
         <v>24</v>
       </c>
@@ -4245,7 +4265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
         <v>25</v>
       </c>
@@ -4268,7 +4288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
         <v>26</v>
       </c>
@@ -4286,12 +4306,12 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="G37" s="43" t="e">
+      <c r="G37" s="43">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="25" t="s">
         <v>27</v>
       </c>
@@ -4314,7 +4334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="25" t="s">
         <v>28</v>
       </c>
@@ -4337,7 +4357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
         <v>29</v>
       </c>
@@ -4360,7 +4380,7 @@
         <v>1.875</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
         <v>31</v>
       </c>

</xml_diff>